<commit_message>
Nuevos datos en las tablas
</commit_message>
<xml_diff>
--- a/Docs/Tablas Lab 4_Juan José Osorio.xlsx
+++ b/Docs/Tablas Lab 4_Juan José Osorio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Thais/Desktop/Universidad/Segundo semestre/EDA/Laboratorios/Laboratorio 4/LabSorts-S06-G06/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176494B1-09EA-F74B-BE42-3B7E90C116B3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CDB9275-DE56-0241-9494-0B50EA9A508C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6340" yWindow="500" windowWidth="14280" windowHeight="15720" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="15400" yWindow="520" windowWidth="14280" windowHeight="15720" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4" sheetId="1" r:id="rId1"/>
@@ -665,7 +665,7 @@
               <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -680,6 +680,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -689,7 +704,7 @@
               <c:f>'Datos Lab4'!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>953.125</c:v>
                 </c:pt>
@@ -803,7 +818,7 @@
               <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -818,6 +833,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -827,7 +857,7 @@
               <c:f>'Datos Lab4'!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1125</c:v>
                 </c:pt>
@@ -940,7 +970,7 @@
               <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -955,6 +985,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -964,7 +1009,7 @@
               <c:f>'Datos Lab4'!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>62.5</c:v>
                 </c:pt>
@@ -979,6 +1024,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1578.125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3484.375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8593.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20281.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84328.125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1490,7 +1550,7 @@
               <c:f>'Datos Lab4'!$A$15:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -1499,6 +1559,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1508,7 +1571,7 @@
               <c:f>'Datos Lab4'!$B$15:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>62031.25</c:v>
                 </c:pt>
@@ -1616,7 +1679,7 @@
               <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>57390.625</c:v>
                 </c:pt>
@@ -1634,7 +1697,7 @@
               <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>57390.625</c:v>
                 </c:pt>
@@ -1741,7 +1804,7 @@
               <c:f>'Datos Lab4'!$A$15:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -1750,6 +1813,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1759,7 +1825,7 @@
               <c:f>'Datos Lab4'!$D$15:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>3359.375</c:v>
                 </c:pt>
@@ -1768,6 +1834,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>67484.375</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>364671.875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2280,7 +2349,7 @@
               <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -2295,6 +2364,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2304,7 +2388,7 @@
               <c:f>'Datos Lab4'!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>953.125</c:v>
                 </c:pt>
@@ -2418,7 +2502,7 @@
               <c:f>'Datos Lab4'!$A$15:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -2427,6 +2511,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2436,7 +2523,7 @@
               <c:f>'Datos Lab4'!$B$15:$B$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>62031.25</c:v>
                 </c:pt>
@@ -2947,7 +3034,7 @@
               <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -2962,6 +3049,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2971,7 +3073,7 @@
               <c:f>'Datos Lab4'!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1125</c:v>
                 </c:pt>
@@ -3085,7 +3187,7 @@
               <c:f>'Datos Lab4'!$A$15:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3094,6 +3196,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3103,7 +3208,7 @@
               <c:f>'Datos Lab4'!$C$15:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>57390.625</c:v>
                 </c:pt>
@@ -3614,7 +3719,7 @@
               <c:f>'Datos Lab4'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3629,6 +3734,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>16000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>32000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>64000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>128000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>256000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3638,7 +3758,7 @@
               <c:f>'Datos Lab4'!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>62.5</c:v>
                 </c:pt>
@@ -3653,6 +3773,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1578.125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3484.375</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8593.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20281.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84328.125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3752,7 +3887,7 @@
               <c:f>'Datos Lab4'!$A$15:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>1000</c:v>
                 </c:pt>
@@ -3761,6 +3896,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>375942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3770,7 +3908,7 @@
               <c:f>'Datos Lab4'!$D$15:$D$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>3359.375</c:v>
                 </c:pt>
@@ -3779,6 +3917,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>67484.375</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="0.00">
+                  <c:v>364671.875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7114,18 +7255,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:D11" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}">
-    <filterColumn colId="1">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-    <filterColumn colId="2">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:D11" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Tamaño de la muestra (ARRAYLIST)" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Insertion Sort [ms]" dataDxfId="8"/>
@@ -7140,7 +7270,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A14:D24" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A14:D24" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}">
     <filterColumn colId="1">
-      <filters blank="1">
+      <filters>
+        <filter val="140,00"/>
+        <filter val="4245234,38"/>
         <filter val="542203,125"/>
         <filter val="62031,25"/>
       </filters>
@@ -7460,8 +7592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B14742-4EBB-4241-AC8A-0E5F24F7BB7B}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="168" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -7556,45 +7688,55 @@
         <v>1578.125</v>
       </c>
     </row>
-    <row r="7" spans="1:4" hidden="1">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>32000</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+      <c r="D7" s="5">
+        <v>3484.375</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" hidden="1">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>64000</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="D8" s="6">
+        <v>8593.75</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" hidden="1">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>128000</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="D9" s="7">
+        <v>20281.25</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" hidden="1">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>256000</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="D10" s="6">
+        <v>53000</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" hidden="1">
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
-        <v>512000</v>
+        <v>375942</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="D11" s="7">
+        <v>84328.125</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="16">
       <c r="A14" s="2" t="s">
@@ -7716,20 +7858,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:4" hidden="1">
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
-        <v>512000</v>
+        <v>375942</v>
       </c>
-      <c r="B24" s="4">
-        <v>140</v>
-      </c>
-      <c r="C24" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
       <c r="D24" s="4">
-        <f t="shared" si="1"/>
-        <v>30</v>
+        <v>364671.875</v>
       </c>
     </row>
   </sheetData>
@@ -7742,6 +7878,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="04b510ef1bc187d79b842c792d256c41">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9049981c3eb1ee76226ec9e2f8ecd7b4" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -7952,22 +8103,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03EB27C0-F9F6-4037-B95E-326B818673EE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7984,21 +8137,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>